<commit_message>
change the order of lessons
</commit_message>
<xml_diff>
--- a/units2.xlsx
+++ b/units2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yasin\vscode__\py_xlrd\auto_unit_setter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFEC2C0-3290-432C-9A65-5FB5BDA40E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36EBB7E-E417-4C90-AE42-D64016EF2DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>rohani</t>
   </si>
   <si>
-    <t>data-stru</t>
-  </si>
-  <si>
     <t>invitee</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>mojiri</t>
   </si>
   <si>
-    <t>english</t>
-  </si>
-  <si>
     <t>azizi</t>
   </si>
   <si>
@@ -171,10 +165,16 @@
     <t>jahangir</t>
   </si>
   <si>
-    <t>az-elec</t>
-  </si>
-  <si>
     <t>wen</t>
+  </si>
+  <si>
+    <t>elec</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>ds</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:F63"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1">
         <v>0.45833333333333331</v>
@@ -544,7 +544,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -552,7 +552,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1">
         <v>0.45833333333333331</v>
@@ -561,27 +561,27 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D4" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -589,116 +589,116 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="D5" s="1">
-        <v>0.45833333333333331</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>0.5625</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D6" s="1">
-        <v>0.6875</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>0.5625</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D7" s="1">
-        <v>0.6875</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1">
-        <v>0.5625</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D8" s="1">
-        <v>0.6875</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1">
-        <v>0.5625</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D9" s="1">
-        <v>0.6875</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.5625</v>
       </c>
       <c r="D10" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -709,16 +709,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.5625</v>
       </c>
       <c r="D11" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -729,16 +729,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.5625</v>
       </c>
       <c r="D12" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
@@ -749,16 +749,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.5625</v>
       </c>
       <c r="D13" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
@@ -769,16 +769,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D14" s="1">
-        <v>0.45833333333333331</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -789,16 +789,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D15" s="1">
-        <v>0.45833333333333331</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -809,16 +809,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D16" s="1">
-        <v>0.45833333333333331</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
@@ -829,16 +829,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D17" s="1">
-        <v>0.45833333333333331</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
@@ -849,82 +849,82 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1">
         <v>0.33333333333333331</v>
       </c>
       <c r="D18" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C19" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D19" s="1">
         <v>0.45833333333333331</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D20" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D20" s="1">
-        <v>0.52083333333333337</v>
-      </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D21" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D21" s="1">
-        <v>0.52083333333333337</v>
-      </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -932,7 +932,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1">
         <v>0.39583333333333331</v>
@@ -944,7 +944,7 @@
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -952,7 +952,7 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1">
         <v>0.5625</v>
@@ -964,7 +964,7 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -972,7 +972,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1">
         <v>0.33333333333333331</v>
@@ -984,7 +984,7 @@
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -992,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
         <v>0.54166666666666663</v>
@@ -1004,7 +1004,7 @@
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="1">
         <v>0.625</v>
@@ -1024,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1">
         <v>0.625</v>
@@ -1044,7 +1044,7 @@
         <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1">
         <v>0.33333333333333331</v>
@@ -1064,7 +1064,7 @@
         <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1072,7 +1072,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C29" s="1">
         <v>0.33333333333333331</v>
@@ -1084,7 +1084,7 @@
         <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1092,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C30" s="1">
         <v>0.41666666666666669</v>
@@ -1104,7 +1104,7 @@
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1112,7 +1112,7 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C31" s="1">
         <v>0.41666666666666669</v>
@@ -1124,7 +1124,7 @@
         <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1">
         <v>0.5625</v>
@@ -1144,7 +1144,7 @@
         <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1152,7 +1152,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1">
         <v>0.5625</v>
@@ -1164,7 +1164,7 @@
         <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,7 +1172,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C34" s="1">
         <v>0.33333333333333331</v>
@@ -1184,7 +1184,7 @@
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1">
         <v>0.33333333333333331</v>
@@ -1204,7 +1204,7 @@
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1">
         <v>0.41666666666666669</v>
@@ -1224,7 +1224,7 @@
         <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1232,7 +1232,7 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C37" s="1">
         <v>0.41666666666666669</v>
@@ -1244,7 +1244,7 @@
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C38" s="1">
         <v>0.5625</v>
@@ -1264,7 +1264,7 @@
         <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1">
         <v>0.5625</v>
@@ -1284,7 +1284,7 @@
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1292,7 +1292,7 @@
         <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C40" s="1">
         <v>0.54166666666666663</v>
@@ -1301,10 +1301,10 @@
         <v>0.625</v>
       </c>
       <c r="E40" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
         <v>14</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C41" s="1">
         <v>0.54166666666666663</v>
@@ -1321,10 +1321,10 @@
         <v>0.625</v>
       </c>
       <c r="E41" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1332,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C42" s="1">
         <v>0.33333333333333331</v>
@@ -1344,7 +1344,7 @@
         <v>13</v>
       </c>
       <c r="F42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,7 +1352,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C43" s="1">
         <v>0.41666666666666669</v>
@@ -1364,7 +1364,7 @@
         <v>13</v>
       </c>
       <c r="F43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1372,7 +1372,7 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C44" s="1">
         <v>0.5625</v>
@@ -1384,7 +1384,7 @@
         <v>13</v>
       </c>
       <c r="F44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C45" s="1">
         <v>0.33333333333333331</v>
@@ -1404,7 +1404,7 @@
         <v>15</v>
       </c>
       <c r="F45" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1412,7 +1412,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C46" s="1">
         <v>0.41666666666666669</v>
@@ -1424,7 +1424,7 @@
         <v>15</v>
       </c>
       <c r="F46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C47" s="1">
         <v>0.5625</v>
@@ -1444,7 +1444,7 @@
         <v>15</v>
       </c>
       <c r="F47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1452,7 +1452,7 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C48" s="1">
         <v>0.33333333333333331</v>
@@ -1464,7 +1464,7 @@
         <v>16</v>
       </c>
       <c r="F48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C49" s="1">
         <v>0.41666666666666669</v>
@@ -1484,7 +1484,7 @@
         <v>16</v>
       </c>
       <c r="F49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C50" s="1">
         <v>0.5625</v>
@@ -1504,7 +1504,7 @@
         <v>16</v>
       </c>
       <c r="F50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C51" s="1">
         <v>0.33333333333333331</v>
@@ -1524,7 +1524,7 @@
         <v>17</v>
       </c>
       <c r="F51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,7 +1532,7 @@
         <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C52" s="1">
         <v>0.41666666666666669</v>
@@ -1544,7 +1544,7 @@
         <v>17</v>
       </c>
       <c r="F52" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1552,7 +1552,7 @@
         <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C53" s="1">
         <v>0.5625</v>
@@ -1564,7 +1564,7 @@
         <v>17</v>
       </c>
       <c r="F53" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C54" s="1">
         <v>0.5625</v>
@@ -1584,7 +1584,7 @@
         <v>13</v>
       </c>
       <c r="F54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55" s="1">
         <v>0.5625</v>
@@ -1604,7 +1604,7 @@
         <v>15</v>
       </c>
       <c r="F55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1612,7 +1612,7 @@
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" s="1">
         <v>0.5625</v>
@@ -1624,7 +1624,7 @@
         <v>16</v>
       </c>
       <c r="F56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
         <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C57" s="1">
         <v>0.5625</v>
@@ -1644,7 +1644,7 @@
         <v>17</v>
       </c>
       <c r="F57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1652,7 +1652,7 @@
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C58" s="1">
         <v>0.5625</v>
@@ -1661,10 +1661,10 @@
         <v>0.6875</v>
       </c>
       <c r="E58" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1672,7 +1672,7 @@
         <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C59" s="1">
         <v>0.39583333333333331</v>
@@ -1684,7 +1684,7 @@
         <v>13</v>
       </c>
       <c r="F59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1692,7 +1692,7 @@
         <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C60" s="1">
         <v>0.39583333333333331</v>
@@ -1704,7 +1704,7 @@
         <v>15</v>
       </c>
       <c r="F60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1712,7 +1712,7 @@
         <v>28</v>
       </c>
       <c r="B61" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C61" s="1">
         <v>0.39583333333333331</v>
@@ -1724,7 +1724,7 @@
         <v>16</v>
       </c>
       <c r="F61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C62" s="1">
         <v>0.39583333333333331</v>
@@ -1744,7 +1744,7 @@
         <v>17</v>
       </c>
       <c r="F62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1752,7 +1752,7 @@
         <v>37</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63" s="1">
         <v>0.39583333333333331</v>
@@ -1761,10 +1761,10 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="E63" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>